<commit_message>
Statistical analysis behavior wue1 and variation per effect
Source data files, jupyter notebook and result files
</commit_message>
<xml_diff>
--- a/stat_results_behavior_lab_wue1.xlsx
+++ b/stat_results_behavior_lab_wue1.xlsx
@@ -669,13 +669,13 @@
         <v>3.622001835880587e-09</v>
       </c>
       <c r="K2">
-        <v>11</v>
+        <v>5.93875107042952</v>
       </c>
       <c r="L2">
-        <v>-5.269682587373573</v>
+        <v>-4.924041030591869</v>
       </c>
       <c r="M2">
-        <v>0.0001322236475421134</v>
+        <v>0.002723474027161755</v>
       </c>
       <c r="N2">
         <v>12</v>
@@ -684,25 +684,25 @@
         <v>-2.737044727144774</v>
       </c>
       <c r="P2">
-        <v>0.009014880497793584</v>
+        <v>0.01802976099558717</v>
       </c>
       <c r="Q2">
-        <v>11</v>
+        <v>5.110877955450509</v>
       </c>
       <c r="R2">
-        <v>-7.773121998251526</v>
+        <v>-7.157419296171146</v>
       </c>
       <c r="S2">
-        <v>4.289107174008809e-06</v>
+        <v>0.0007545837546247165</v>
       </c>
       <c r="T2">
-        <v>11</v>
+        <v>8.770028048607942</v>
       </c>
       <c r="U2">
-        <v>2.761499730337956</v>
+        <v>2.682430007698034</v>
       </c>
       <c r="V2">
-        <v>0.009253087196378748</v>
+        <v>0.02566849408417354</v>
       </c>
       <c r="W2">
         <v>10</v>
@@ -711,16 +711,16 @@
         <v>-5.132811455314671</v>
       </c>
       <c r="Y2">
-        <v>0.0002211809837109243</v>
+        <v>0.0004423619674218486</v>
       </c>
       <c r="Z2">
-        <v>11</v>
+        <v>5.493591994660114</v>
       </c>
       <c r="AA2">
-        <v>-6.868552608923256</v>
+        <v>-6.36966040925418</v>
       </c>
       <c r="AB2">
-        <v>1.348591744847055e-05</v>
+        <v>0.0009899094687557135</v>
       </c>
       <c r="AC2">
         <v>20.89426321709787</v>
@@ -797,13 +797,13 @@
         <v>2.140454257535751e-06</v>
       </c>
       <c r="K3">
-        <v>11</v>
+        <v>8.902919501762254</v>
       </c>
       <c r="L3">
-        <v>2.725627684781509</v>
+        <v>2.871543685029924</v>
       </c>
       <c r="M3">
-        <v>0.009865981517707461</v>
+        <v>0.01863121819846281</v>
       </c>
       <c r="N3">
         <v>12</v>
@@ -812,25 +812,25 @@
         <v>1.906945981017726</v>
       </c>
       <c r="P3">
-        <v>0.04037373686858424</v>
+        <v>0.08074747373716848</v>
       </c>
       <c r="Q3">
-        <v>11</v>
+        <v>10.35639372068132</v>
       </c>
       <c r="R3">
-        <v>6.488372789072021</v>
+        <v>6.712406019215754</v>
       </c>
       <c r="S3">
-        <v>2.249389356009045e-05</v>
+        <v>4.458652923885313e-05</v>
       </c>
       <c r="T3">
-        <v>11</v>
+        <v>10.5850986279771</v>
       </c>
       <c r="U3">
-        <v>-1.012616297541351</v>
+        <v>-1.043349814830959</v>
       </c>
       <c r="V3">
-        <v>0.1664996168753807</v>
+        <v>0.3200291738785926</v>
       </c>
       <c r="W3">
         <v>10</v>
@@ -839,16 +839,16 @@
         <v>5.682208945087392</v>
       </c>
       <c r="Y3">
-        <v>0.000101610868251039</v>
+        <v>0.0002032217365020781</v>
       </c>
       <c r="Z3">
-        <v>11</v>
+        <v>10.90056535870338</v>
       </c>
       <c r="AA3">
-        <v>5.891001078573217</v>
+        <v>5.927053182217047</v>
       </c>
       <c r="AB3">
-        <v>5.223617077380275e-05</v>
+        <v>0.0001028756689983914</v>
       </c>
       <c r="AC3">
         <v>16.45706145706147</v>

</xml_diff>